<commit_message>
no new just XLSX
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -2,15 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6120" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -50,7 +49,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -413,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -424,170 +423,1161 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>IND8-12G-A</t>
+          <t>ABM7-25.000MHZ-D2Y-T ABRACON</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>IND8-12G-A</t>
+          <t>ABM7-25.000MHZ-D2Y</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Индикат.лампа: LED; выпуклый; 12ВDC; Отв: Ø8,2мм; IP40; под пайку</t>
+          <t>Резонатор: керамический; 25МГц; ±20ppm; 18пФ; SMD; 6x3,5x1,4мм</t>
         </is>
       </c>
       <c r="D1" t="n">
-        <v>0.00443</v>
+        <v>0.00012</v>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@aea78e09d2abae4de0b55df4a687b93507857be1/_cdn_/6B/D4/50/00/0/347574_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@b052f1daf4619ca8fc7fb4ddc5a3c4b3a8c2a672/_cdn_/42/2E/00/00/0/57892_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/ind8-12g-a/led-panelnye-indikatory/ninigi/</t>
+          <t>//www.tme.eu/ru/details/abm7-25.000mhz-d2y/kvartsevye-rezonatory-smd/abracon/abm7-25-000mhz-d2y-t/</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>{'Тип индик. лампы': 'LED', 'Вид индикатора': 'выпуклый', 'Цвет диодa LED': 'зеленый', 'Рабочее напряжение': '12В DC', 'Размер монтажного отверстия': 'Ø8,2мм', 'Класс защиты': 'IP40', 'Выводы': 'под пайку', 'Материал корпуса': 'металл', 'Диаметр диода LED': '5мм', 'Рабочая температура': '-25...70°C', 'Цвет': 'серебристый'}</t>
+          <t>{'Тип резонатора': 'керамический', 'Частота': '25МГц', 'Емкость': '18пФ', 'Монтаж': 'SMD', 'Нестабильность частоты': '±30ppm', 'Рабочая температура': '-40...85°C', 'Размеры корпуса': '6x3,5x1,4мм', 'Долговременная стабильность': '±5ppm/год'}</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/083b9525773c3812c05eddbfb7453428/abm7.pdf</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Световые индикаторы, для монтажа на панель. Тип индик. лампы LED, Вид индикатора выпуклый, цвет свечения диодa зеленый, Рабочее напряжение 12В постоянного тока, Размер монтажного отверстия диам. 8,2мм, Класс защиты IP40, Выводы под пайку, Материал корпуса металл, диаметр диода 5мм, Рабочая температура -25...70°C, Цвет серебристый, рабочие температуры от -40 до 80°С, используется в качестве светового индикатора на панели приборов и в модульных переключателях, применяется в радиоэлектронных приборах общепромышленного назначения.</t>
+          <t xml:space="preserve"> Осцилляторы тактовых импульсов на основе пьезоэлектрического кварцевого кристалла. Частота 25МГц, Емкость 18пФ, Монтаж на поверхность печатной платы, Нестабильность частоты +\- 30ppm, Рабочая температура -40...85°C, Размеры корпуса 6x3,5x1,4мм, Долговременная стабильность +\- 5ppm/год, рабочий диапазон температур от -40 до 85 гр, предназначено для радиоэлектронной аппаратуры общепромышленного назначения.</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>Тип индик. лампы LED</t>
+          <t>Тип резонатора керамический</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>NINIGI</t>
+          <t>ABRACON</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>ABM7-25.000MHZ-D2Y-T</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>IND8-12G-B</t>
+          <t>22260120</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>IND8-12G-B</t>
+          <t>22260120</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Индикат.лампа: LED; вогнутый; 12ВDC; Отв: Ø8,2мм; IP40; под пайку</t>
+          <t>Разъем: M8; "папа"; PIN: 3; прямой; на провод; вилка; внешняя резьба</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>0.00491</v>
+        <v>0.011</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@5a8107c06faff59232aab138295ce209a729c452/_cdn_/39/84/50/00/0/346259_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@09dc8ce9646bd617bcef62ae25e248a4b0989061/_cdn_/8E/9D/60/00/0/449000_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/ind8-12g-b/led-panelnye-indikatory/ninigi/</t>
+          <t>//www.tme.eu/ru/details/22260120/razemy-m8/lapp/</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>{'Тип индик. лампы': 'LED', 'Вид индикатора': 'вогнутый', 'Цвет диодa LED': 'зеленый', 'Рабочее напряжение': '12В DC', 'Размер монтажного отверстия': 'Ø8,2мм', 'Класс защиты': 'IP40', 'Выводы': 'под пайку', 'Материал корпуса': 'металл', 'Диаметр диода LED': '5мм', 'Рабочая температура': '-25...70°C', 'Цвет': 'серебристый'}</t>
+          <t>{'Тип разъема': 'M8', 'Вид разъемов': '"папа"', 'Кол-во выводов': '3', 'Пространственная ориентация': 'прямой', 'Механический монтаж': 'на провод', 'Разъем': 'вилка', 'Фиксация разъема': 'внешняя резьба', 'Максимальный ток': '4А', 'Электрический монтаж': 'зажим под винт', 'Класс защиты': 'IP67', 'Номинальное напряжение': '40В', 'Внешний диаметр провода': '3,5...5мм', 'Сечение провода': '0,14...0,5мм&lt;sup&gt;2&lt;/sup&gt;'}</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/5754a86500aa681c3486cf540fa40442/22260120.pdf</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Световые индикаторы, для монтажа на панель. Тип индик. лампы LED, Вид индикатора вогнутый, цвет свечения диодa зеленый, Рабочее напряжение 12В постоянного тока, Размер монтажного отверстия диам. 8,2мм, Класс защиты IP40, Выводы под пайку, Материал корпуса металл, диаметр диода 5мм, Рабочая температура -25...70°C, Цвет серебристый, рабочие температуры от -40 до 80°С, используется в качестве светового индикатора на панели приборов и в модульных переключателях, применяется в радиоэлектронных приборах общепромышленного назначения.</t>
+          <t xml:space="preserve"> Штепсельные цилиндрические разъемы для монтажа на .... Тип разъема M8, Вид разъемов штепсель-вилка, Кол-во выводов 3, Пространственная ориентация прямой, Механический монтаж на провод, Разъем вилка, Фиксация разъема внешняя резьба, Максимальный ток 4А, Электрический монтаж зажим под винт, Класс защиты IP67, Номинальное напряжение 40В, Внешний диаметр провода 3,5...5мм, Сечение провода 0,14...0,5кв. мм, предназначены для использования в радиоэлектронном оборудовании общепромышленного назначения.</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Тип индик. лампы LED</t>
+          <t>Тип разъема M8</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>NINIGI</t>
+          <t>LAPP</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>IND8-12G-A</t>
+          <t>22260120</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>IND8-12R-A</t>
+          <t>60630-00002-00 TESA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>IND8-12R-A</t>
+          <t>TESA-60630-50-50M</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Индикат.лампа: LED; выпуклый; 12ВDC; Отв: Ø8,2мм; IP40; под пайку</t>
+          <t>Лента: ремонтная; W: 50мм; L: 50м; Thk: 30мкм; серый; акриловый; 3%</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0.0046</v>
+        <v>0.3358</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@033475c84016b50f71ccc1b588c94a4af2edcee1/_cdn_/F5/2E/60/00/0/451167_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@41eb8281927b049b004ab5a3efe6f5760e443fe9/_cdn_/8B/F1/A0/00/0/663480_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>www.tme.eu/ru/details/ind8-12r-a/led-panelnye-indikatory/ninigi/</t>
+          <t>//www.tme.eu/ru/details/tesa-60630-50-50m/lenty-remontnye/tesa/60630-00002-00/</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>{'Тип индик. лампы': 'LED', 'Вид индикатора': 'выпуклый', 'Цвет диодa LED': 'красный', 'Рабочее напряжение': '12В DC', 'Размер монтажного отверстия': 'Ø8,2мм', 'Класс защиты': 'IP40', 'Выводы': 'под пайку', 'Материал корпуса': 'металл', 'Диаметр диода LED': '5мм', 'Рабочая температура': '-25...70°C', 'Цвет': 'серебристый'}</t>
+          <t>{'Тип ленты': 'ремонтная', 'Ширина': '50мм', 'Длина': '50м', 'Толщина': '30мкм', 'Цвет': 'серый', 'Вид клея': 'акриловый', 'Материал носителя': 'алюминий', 'Рабочая температура': 'макс. 160°C', 'Адгезия к стали': '8Н/cм', 'Устойчивы к': 'растяжению', 'Применение ленты': 'connecting and sealing thermal insulation and wires', 'Характеристики лент': 'хорошая электропроводность'}</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t xml:space="preserve"> Световые индикаторы, для монтажа на панель. Тип индик. лампы LED, Вид индикатора выпуклый, цвет свечения диодa красный, Рабочее напряжение 12В постоянного тока, Размер монтажного отверстия диам. 8,2мм, Класс защиты IP40, Выводы под пайку, Материал корпуса металл, диаметр диода 5мм, Рабочая температура -25...70°C, Цвет серебристый, рабочие температуры от -40 до 80°С, используется в качестве светового индикатора на панели приборов и в модульных переключателях, применяется в радиоэлектронных приборах общепромышленного назначения.</t>
+          <t xml:space="preserve"> Тип ленты ремонтная, в рулоне шириной 50мм, длиной 50м, толщина пленки 30мкм, Цвет серый, Вид клея акриловый, ленты изготовлены алюминий, Рабочая температура до 160°C, Адгезия к стали 8Н/cм, Устойчивы к растяжению, Применение ленты connecting and sealing thermal insulation and wires, Характеристики лент хорошая электропроводность. Применяется при проведении монтажных работ, в качестве упаковочной ленты, для складских нужд.</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Тип индик. лампы LED</t>
+          <t>Тип ленты ремонтная</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>NINIGI</t>
+          <t>TESA</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>IND8-12G-B</t>
+          <t>60630-00002-00</t>
         </is>
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>22260120 LAPP</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>22260120</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Разъем: M8; "папа"; PIN: 3; прямой; на провод; вилка; внешняя резьба</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>0.011</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@09dc8ce9646bd617bcef62ae25e248a4b0989061/_cdn_/8E/9D/60/00/0/449000_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/22260120/razemy-m8/lapp/</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>{'Тип разъема': 'M8', 'Вид разъемов': '"папа"', 'Кол-во выводов': '3', 'Пространственная ориентация': 'прямой', 'Механический монтаж': 'на провод', 'Разъем': 'вилка', 'Фиксация разъема': 'внешняя резьба', 'Максимальный ток': '4А', 'Электрический монтаж': 'зажим под винт', 'Класс защиты': 'IP67', 'Номинальное напряжение': '40В', 'Внешний диаметр провода': '3,5...5мм', 'Сечение провода': '0,14...0,5мм&lt;sup&gt;2&lt;/sup&gt;'}</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/5754a86500aa681c3486cf540fa40442/22260120.pdf</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Штепсельные цилиндрические разъемы для монтажа на .... Тип разъема M8, Вид разъемов штепсель-вилка, Кол-во выводов 3, Пространственная ориентация прямой, Механический монтаж на провод, Разъем вилка, Фиксация разъема внешняя резьба, Максимальный ток 4А, Электрический монтаж зажим под винт, Класс защиты IP67, Номинальное напряжение 40В, Внешний диаметр провода 3,5...5мм, Сечение провода 0,14...0,5кв. мм, предназначены для использования в радиоэлектронном оборудовании общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Тип разъема M8</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>LAPP</t>
+        </is>
+      </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>IND8-12R-A</t>
-        </is>
-      </c>
-    </row>
+          <t>22260120</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>9204260000 WEIDMÜLLER</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>WDM-AM16/B</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Лезвие; Назначение: WDM-AM16</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@bc6e0cb82efd971288d00c26985edc76b4745b91/_cdn_/31/66/80/00/0/550419_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/wdm-am16_b/ustroistva-dlia-sniatiia-izoliatsii/weidmuller/9204260000/</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>{'Запасной комплект': 'лезвие', 'Назначение': 'WDM-AM16'}</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/40285549ddd80d86a557911cf51fb121/WDM-AM16_B.pdf</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>WEIDMÜLLER</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>9204260000</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>3-640427-4 TE\\xa0Connectivity</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>281190-15-0 ACV</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>RAM-40.144</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Рамка для магнитолы; Smart; 1 DIN; антрацит</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0493</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@86ec394e486219c0aa59f3096f3aef6182292e3b/_cdn_/92/9A/50/00/0/370985_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/ram-40.144/ramki-dlia-radio/acv/281190-15-0/</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>{'Тип аксессуаров car audio': 'рамка для магнитолы', 'Применение (марка автомобиля)': 'Smart', 'Применение (модель автомобиля)': 'Smart Roadster', 'Версия автомобильных аксессуаров': '1 DIN', 'Цвет': 'антрацит'}</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>Тип аксессуаров car audio рамка для магнитолы</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>ACV</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>281190-15-0</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>DS3106A22-14P AMPHENOL</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>DS3106A22-14P</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Разъем: круглый; Серия: DS/MS; вилка; "папа"; PIN: 19; посеребренные</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>0.0761</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@1198dd75fe36a3d79533e97d4cd74bf1753fbe2a/_cdn_/A0/84/50/00/0/346122_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/ds3106a22-14p/razemy-mil-c-5015/amphenol/</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>{'Тип разъема': 'круглый', 'Серия разъема': 'DS/MS', 'Разъем': 'вилка', 'Вид разъемов': '"папа"', 'Кол-во выводов': '19', 'Фиксация разъема': 'резьбовая', 'Покрытие контакта': 'посеребренные', 'Механический монтаж': 'на провод', 'Электрический монтаж': 'пайка', 'Номинальный ток': '13А', 'Корпус': 'размер 22', 'Материал корпуса': 'алюминий', 'Цвет': 'оливково-серый', 'Соответствуют норме': 'MIL-C-5015', 'Конфигурация выводов разъема': '22-14', 'Пространственная ориентация': 'прямой', 'Номинальное напряжение': '700В DC', 'Сечение провода': '0,5...1,5мм&lt;sup&gt;2&lt;/sup&gt;'}</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/31dc9f8ad5921d4f99c2e8b4e83d3d5e/ds3106a.pdf</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Штепсельные цилиндрические разъемы, серии DS/MS, для монтажа на проводники, c 19 контактами c конфигурацией выводов 22-14. Номинальное напряжение 700В постоянного тока, номинальный ток 13А, контакты изготовлены из медного сплава с гальваническим покрытием, материал корпуса полиамид, рабочие температуры от -40 до 105°С, предназначены для радиоэлектронного оборудования общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Тип разъема круглый</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>AMPHENOL</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>DS3106A22-14P</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DS3101A22-14S AMPHENOL</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>DS3101A22-14S</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Разъем: круглый; Серия: DS/MS; вилка; "мама"; PIN: 19; посеребренные</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0834</v>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@9b2ca354340e4defc50dc4801809e3fa9cfca2d1/_cdn_/9B/4D/50/00/0/382137_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/ds3101a22-14s/razemy-mil-c-5015/amphenol/</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>{'Тип разъема': 'круглый', 'Серия разъема': 'DS/MS', 'Разъем': 'вилка', 'Вид разъемов': '"мама"', 'Кол-во выводов': '19', 'Фиксация разъема': 'резьбовая', 'Покрытие контакта': 'посеребренные', 'Механический монтаж': 'на провод', 'Электрический монтаж': 'пайка', 'Номинальный ток': '13А', 'Корпус': 'размер 22', 'Материал корпуса': 'алюминий', 'Цвет': 'оливково-серый', 'Соответствуют норме': 'MIL-C-5015', 'Конфигурация выводов разъема': '22-14', 'Пространственная ориентация': 'прямой', 'Номинальное напряжение': '700В DC', 'Сечение провода': '0,5...1,5мм&lt;sup&gt;2&lt;/sup&gt;'}</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/dabf368933cd1407b018bd66e703bede/ds3101a.pdf</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Штепсельные цилиндрические разъемы, серии DS/MS, для монтажа на проводники, c 19 контактами c конфигурацией выводов 22-14. Номинальное напряжение 700В постоянного тока, номинальный ток 13А, контакты изготовлены из медного сплава с гальваническим покрытием, материал корпуса полиамид, рабочие температуры от -40 до 105°С, предназначены для радиоэлектронного оборудования общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Тип разъема круглый</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>AMPHENOL</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>DS3101A22-14S</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2097370 BOSSARD</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>B3.5X16/BN14065</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Винт; для металла; 3,5x16; Головка: цилиндрическая; Pozidriv; цинк</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.0012</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@d0843c2ac23557606291b561fc30ae64b38dc823/_cdn_/F9/B7/10/00/1/97183_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/b3.5x16_bn14065/shurupy/bossard/2097370/</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>{'Тип крепежного элемента': 'винт', 'Применение винтов': 'для металла', 'Резьба': '3,5', 'Длина': '16мм', 'Вид головки': 'цилиндрическая', 'Вид шлица': 'Pozidriv', 'Материал': 'сталь', 'Материал покрытия': 'цинк', 'Норма BN': '14065', 'Размер шлица': 'PZ2', 'Диаметр головки': '6,9мм', 'Норма DIN': '7981F', 'Норма ISO': '7049'}</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/887a3efdf0c2d0aa0ca2eab23f7f6232/BN14065.pdf</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Винты с круглой головкой, с крестообразным шлицем.  Применение винтов для металла, Резьба 3,5, Длина 16мм, Вид головки цилиндрическая, Вид шлица Pozidriv, Материал легированная сталь марки Ст.35, цинк, Норма BN 14065, Размер шлица PZ2, Диаметр головки 6,9мм, Норма DIN 7981F, Норма ISO 7049. Предназначены для использования в качестве крепежа в изделиях общей промышленности.</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Тип крепежного элемента винт</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>BOSSARD</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>2097370</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CLG-150-36A MEAN\\xa0WELL</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>3625/10\\xa0(100FT) 3M</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>50434 QOLTEC</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>QOLTEC-50434</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Кабель; DisplayPort 1.1; 1,8м; черный</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0747</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@e0256b883044b04b5645a13ef1533a33364b7a4d/_cdn_/C8/DF/80/00/0/589196_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/qoltec-50434/kabeli-i-adaptery-hdmi-dvi-displayport/qoltec/50434/</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>{'Тип соединительного кабеля': 'DisplayPort - DisplayPort', 'Версия': 'DisplayPort 1.1', 'Конструкция кабеля / переходника': 'вилка mini DisplayPort', 'Длина кабеля': '1,8м', 'Цвет изоляции': 'черный', 'Характеристики соединительного кабеля': 'обеспечивает 3D с разрешением до 1080p'}</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/f5d54b02c39c9f9d3c96984560c13464/50434.pdf</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Кабельные сборки из проводников электрических, изолированных, оснащенных соединителями. Тип соединительного кабеля DisplayPort - DisplayPort, Версия DisplayPort 1.1, Конструкция кабеля / переходника вилка mini DisplayPort, Длина кабеля 1,8м, Цвет изоляции черный, Характеристики соединительного кабеля обеспечивает 3D с разрешением до 1080p. Предназначены для передачи низковольтного, дифференциального сигнала в радиоэлектронном оборудовании общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Тип соединительного кабеля DisplayPort - DisplayPort</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>QOLTEC</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>50434</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>3RG4031-6KD00-2AA0 PEPPERL+FUCHS</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>9140006257 HARTING</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>09140006257</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Контакт; "мама"; Han Modular Pneumatic; на пневмопровод Ø3мм</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0.00063</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@25cd42f5b39c2ff64fbd6ad4ee866e8c5338e06d/_cdn_/8E/DD/00/00/0/56808_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/09140006257/razemy-harting/harting/</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>{'Тип разъема': 'пневматический', 'Разъем': 'контакт', 'Вид разъемов': '"мама"', 'Серия разъема': 'Han Modular Pneumatic', 'Применяются с разъемами': 'на пневмопровод Ø3мм', 'Ресурс': '500 циклов', 'Версия разъема': 'с запорным клапаном', 'Материал': 'Delrin', 'Engineering PN': 'Pneumatic contact fem. with valve 3,0 mm', 'Alias': '09 14 000 6257'}</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/012c008f0480f36a2b54fa17d9b838e9/TB_09140006257_BL01_R413153.pdf</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Параметры без описания: Тип разъема пневматический, Разъем контакт, Вид разъемов штепсель-розетка, Серия разъема Han Modular Pneumatic, Применяются с разъемами на пневмопровод диам. 3мм, Ресурс 500 циклов, Версия разъема с запорным клапаном, Материал Delrin, Engineering PN Pneumatic contact fem. with valve 3,0 mm, Alias 09 14 000 6257.</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Тип разъема пневматический</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>HARTING</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>09140006257</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>9310062701 HARTING</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>09310062701</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Разъем: прямоугольный; "мама"; Han HsB; PIN: 6; 6+PE; размер 16В</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>0.09046999999999999</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@9d6976c9d69b2e133201e6d701b103ee7b2bf798/_cdn_/9C/5E/50/00/0/386505_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/09310062701/razemy-harting/harting/</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>{'Тип разъема': 'прямоугольный', 'Вид разъемов': '"мама"', 'Серия разъема': 'Han HsB', 'Кол-во выводов': '6', 'Конфигурация выводов разъема': '6+PE', 'Корпус': 'размер 16В', 'Электрический монтаж': 'зажим под винт', 'Номинальный ток': '35А', 'Номинальное напряжение': '690В', 'Ресурс': '500 циклов', 'Класс горючести': 'UL94V-0', 'Покрытие контакта': 'посеребренные', 'Толщина покрытия': '3мкм', 'Материал контакта': 'сплав меди', 'Материал изолятора': 'поликарбонат', 'Рабочая температура': '-40...125°C', 'Alias': '09 31 006 2701', 'Engineering PN': 'Han 6HsB-F-S', 'Крепление вставки': '77,5x27мм', 'Сечение провода': '6мм&lt;sup&gt;2&lt;/sup&gt;'}</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/a37cd13c1e0a481277d1c4efec401640/09310062701.pdf</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Штепсельные разъемы типа прямоугольный, серии Han HsB, для монтажа с помощью винтов на корпус или панель, c 6 контактами c конфигурацией выводов 6+PE. Номинальное напряжение 690В, номинальный ток 35А, контакты изготовлены из медного сплава с гальваническим покрытием, материал корпуса полиамид, рабочие температуры от -40 до 105°С, предназначены для радиоэлектронного оборудования общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>Тип разъема прямоугольный</t>
+        </is>
+      </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>HARTING</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>09310062701</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>9310062601 HARTING</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>09310062601</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Разъем: прямоугольный; "папа"; Han HsB; PIN: 6; 6+PE; размер 16В</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0853</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@c622b441531ec1494bdc5d30630fc5b9bac8c7d2/_cdn_/8C/5E/50/00/0/386504_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/09310062601/razemy-harting/harting/</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>{'Тип разъема': 'прямоугольный', 'Вид разъемов': '"папа"', 'Серия разъема': 'Han HsB', 'Кол-во выводов': '6', 'Конфигурация выводов разъема': '6+PE', 'Корпус': 'размер 16В', 'Электрический монтаж': 'зажим под винт', 'Номинальный ток': '35А', 'Номинальное напряжение': '690В', 'Ресурс': '500 циклов', 'Класс горючести': 'UL94V-0', 'Покрытие контакта': 'посеребренные', 'Толщина покрытия': '3мкм', 'Материал контакта': 'сплав меди', 'Материал изолятора': 'поликарбонат', 'Рабочая температура': '-40...125°C', 'Alias': '09 31 006 2601', 'Engineering PN': 'Han 6HsB-M-S', 'Крепление вставки': '77,5x27мм', 'Сечение провода': '6мм&lt;sup&gt;2&lt;/sup&gt;'}</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/f3758f16aeb71994f03017b1c3e80e3f/09310062601.pdf</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Штепсельные разъемы типа прямоугольный, серии Han HsB, для монтажа с помощью винтов на корпус или панель, c 6 контактами c конфигурацией выводов 6+PE. Номинальное напряжение 690В, номинальный ток 35А, контакты изготовлены из медного сплава с гальваническим покрытием, материал корпуса полиамид, рабочие температуры от -40 до 105°С, предназначены для радиоэлектронного оборудования общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>Тип разъема прямоугольный</t>
+        </is>
+      </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>HARTING</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>09310062601</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>19300061540 HARTING</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>19300061540</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Корпус: для разъемов HDC; Мат-л корп: сплав алюминия; на провод</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0.1095</v>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@2eed10bc2977162a76b2fcd15d7a2e80ab7fcbbc/_cdn_/30/6C/50/00/0/378371_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/19300061540/razemy-prochie-harting/harting/</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>{'Тип корпуса': 'для разъемов HDC', 'Материал корпуса': 'сплав алюминия', 'Серия разъема': 'Han B', 'Механический монтаж': 'на провод', 'Корпус': 'размер 6В', 'Фиксация разъема': 'на защелке', 'Alias': '19 30 006 1540', 'Engineering PN': 'Han B Hood Side Entry LC 2 M20', 'Резьба кабельного ввода': 'M20', 'Крепление вставки': '44x27мм', 'Рабочая температура': '-40...125°C', 'Пространственная ориентация': 'угловой', 'Класс защиты': 'IP65', 'Кол-во отверстий в кабельном вводе': '1'}</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/0b383ce99b31e4b5d9df09232bcb4351/19300061540.pdf</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Части штепсельных разъёмов — корпусы для разъемов HDC, Материал корпуса сплав алюминия,  серии Han B, Механический монтаж на провод, типоразмер 6В, Фиксация разъема на защелке, Alias 19 30 006 1540, Engineering PN Han B Hood Side Entry LC 2 M20, Резьба кабельного ввода M20, Крепление вставки 44x27мм, Рабочая температура -40...125°C, Пространственная ориентация угловой, Класс защиты IP65, Кол-во отверстий в кабельном вводе 1, предназначены для изготовления штепсельного разъёма.</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Тип корпуса для разъемов HDC</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>HARTING</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>19300061540</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>216X8 DREMEC</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>TFM-M4X8/DR216</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Дистанцирующая стойка с резьбой; Внутр.резьба: M4; 8мм; латунь</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>0.00276</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@80c083acc187caa849b7ba7fcf530a270488a832/_cdn_/93/6B/00/00/0/46649_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/tfm-m4x8_dr216/elementy-distantsionnye-metallicheskie/dremec/216x8/</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>{'Тип распорнои стойки': 'дистанцирующая стойка с резьбой', 'Внутренняя резьба': 'M4', 'Расстояние между платами': '8мм', 'Внешняя резьба': 'M4', 'Форма стойки': 'шестигранная', 'Материал': 'латунь', 'Материал покрытия': 'никель', 'Размер ключа': '7мм', 'Характеристики механических элементов': 'с внутренней и внешней резьбой'}</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/32d76453d25a68678ccac510b19a0e43/cb958a517a0baea06d47cef058fff4e3 7.pdf</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Стойки дистанцирующие для монтажа печатных плат, изготовленные из ... . Внутренняя резьба M4, высота стойки 8мм, Внешняя резьба M4, Форма стойки шестигранная, Материал латунь, Материал покрытия никель, размер под ключ 7мм, стойки оснащены внутренней и внешней резьбой. Предназначены для совместного монтажа с печатными платами в корпуса электротехнических сборок.</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Тип распорнои стойки дистанцирующая стойка с резьбой</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>DREMEC</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>216X8</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>388/4.2X4 DREMEC</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>DR388/4.2X4</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Дистанцирующая стойка; цилиндрическая; полиамид; Дл: 4мм</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>0.00019</v>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@ccbda7ec6315b36b72822d4ba7b7de1f3c7d11fd/_cdn_/15/6E/00/00/0/58961_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/dr388_4.2x4/plastmassovye-distantsionnye-vtulki/dremec/388-4-2x4/</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>{'Тип распорнои стойки': 'дистанцирующая стойка', 'Форма стойки': 'цилиндрическая', 'Материал': 'полиамид', 'Расстояние между платами': '4мм', 'Внешний диаметр': '8мм', 'Внутренний диаметр': '4,2мм', 'Цвет': 'черный', 'Рабочая температура': 'макс. 110°C'}</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/451757bfa0cf89650334b0f101e3f2bd/Dremec_13.pdf</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Стойки дистанцирующие для монтажа печатных плат, изготовленные из ... .Форма стойки цилиндрическая, Материал полиамид, высота стойки 4мм, Внешний диаметр 8мм, Внутренний диаметр 4,2мм, Цвет черный, Рабочая температура до 110°C. Предназначены для совместного монтажа с печатными платами в корпуса электротехнических сборок.</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Тип распорнои стойки дистанцирующая стойка</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>DREMEC</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>388/4.2X4</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>388/4.2X8 DREMEC</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>DR388/4.2X8</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Дистанцирующая стойка; цилиндрическая; полиамид; Дл: 8мм</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>0.00039</v>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@ccbda7ec6315b36b72822d4ba7b7de1f3c7d11fd/_cdn_/15/6E/00/00/0/58961_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/dr388_4.2x8/plastmassovye-distantsionnye-vtulki/dremec/388-4-2x8/</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>{'Тип распорнои стойки': 'дистанцирующая стойка', 'Форма стойки': 'цилиндрическая', 'Материал': 'полиамид', 'Расстояние между платами': '8мм', 'Внешний диаметр': '8мм', 'Внутренний диаметр': '4,2мм', 'Цвет': 'черный', 'Рабочая температура': 'макс. 110°C'}</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/451757bfa0cf89650334b0f101e3f2bd/Dremec_13.pdf</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Стойки дистанцирующие для монтажа печатных плат, изготовленные из ... .Форма стойки цилиндрическая, Материал полиамид, высота стойки 8мм, Внешний диаметр 8мм, Внутренний диаметр 4,2мм, Цвет черный, Рабочая температура до 110°C. Предназначены для совместного монтажа с печатными платами в корпуса электротехнических сборок.</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Тип распорнои стойки дистанцирующая стойка</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>DREMEC</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>388/4.2X8</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>DVA.4-20-10-M6-18-55 ELESA+GANTER</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>794610-1 TE\\xa0Connectivity</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>DLA100B1200LB-TUB IXYS</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>DLA100B1200LB-TUB</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>Однофазный выпрямительный мост; Urmax: 1,2кВ; If: 124А; Ifsm: 400А</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>0.00804</v>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@f61d6bbf2015e3fb81c4d6ee6d7707ea7fddaee7/_cdn_/7D/F1/B0/00/0/729047_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/dla100b1200lb-tub/odnofaznye-mosty-diodnye-smd-tht/ixys/</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>{'Тип полупроводникового элемента': 'однофазный выпрямительный мост', 'Обратное напряжение макс.': '1,2кВ', 'Падение напряжения макс.': '1,23В', 'Прямой ток': '124А', 'Импульсный ток': '400А', 'Корпус': 'SMPD', 'Электрический монтаж': 'SMT'}</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/0869e11af82c1ad835122174179d37de/DLA100B1200LB.pdf</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Диоды в сборке выполненной из 4 диодов собранных по схеме однофазный выпрямительный мост. Обратное напряжение до 1,2кВ, Прямой ток 124А, Импульсный ток 400А, тип корпуса SMPD, вид монтажа на поверхность печатной платы, рабочие температуры от -40 до 150°С, предназначены для использования в радиоэлектронном оборудовании общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>Тип полупроводникового элемента однофазный выпрямительный мост</t>
+        </is>
+      </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>IXYS</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>DLA100B1200LB-TUB</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>3534 KEYSTONE</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>KEYS3534</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>Наконечник: плоский; 2,8мм; 0,5мм; "мама"; THT; латунь; луженые</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>0.00018</v>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/fit/640x480/n@75bdbcddd41f4aba1d9da4a7eb68f7169a9ca33f/_cdn_/10/B1/70/00/0/465665_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/keys3534/paechnye-shtifty-pcb/keystone/3534/</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>{'Тип разъема': 'плоский', 'Ширина': '2,8мм', 'Толщина': '0,5мм', 'Вид наконечника': '"мама"', 'Электрический монтаж': 'THT', 'Материал контакта': 'латунь', 'Покрытие контакта': 'луженые', 'Длина': '11,2мм', 'Пространственная ориентация': 'прямой'}</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/44e0eada79ff6f8ea538730061a09197/3534.PDF</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Части штепсельных разъёмов — контакты типа ..., изготовлены из медного сплава(фосфористая бронза). для установки в разъёмы плоский, Ширина 2,8мм, Толщина 0,5мм, Вид наконечника штепсель-розетка, монтаж с проводниками в отверстия печатной платы, Материал контакта латунь, гальваническое покрытие из луженые, Длина 11,2мм, Пространственная ориентация прямой, номинальный ток 3 А, предназначены  для изготовления штепсельного разъёма.</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>Тип разъема плоский</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>KEYSTONE</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>3534</t>
+        </is>
+      </c>
+    </row>
+    <row r="26"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
New BD data 14012021
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,62 +421,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>P15030201E.BL</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>IT-P15030201E.BL</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Заглушка; серый</t>
-        </is>
-      </c>
-      <c r="D1" t="n">
-        <v>0.0011</v>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>https://ce8dc832c.cloudimg.io/fit/640x480/fwk@970ea0de70e253475be98a919bd8eb2f6028aebf/_cdn_/07/59/70/00/0/497008_1.jpg?mark_url=_tme-wrk_%2Ftme_new.png&amp;mark_pos=center&amp;mark_size=100pp</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>//www.tme.eu/ru/details/it-p15030201e.bl/aksessuary-k-korpusam-na-din-reiku/italtronic/p15030201e-bl/</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>{'Тип аксессуаров для корпусов': 'заглушка', 'Применение': '3M Modulbox XTS Compact', 'Цвет': 'серый'}</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>https://www.tme.eu/Document/3b86e6b0a6b0f38640ae5a047fddd943/p15020201e_bl.pdf</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Тип аксессуаров для корпусов заглушка</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>ITALTRONIC</t>
-        </is>
-      </c>
-      <c r="L1" t="inlineStr">
-        <is>
-          <t>P15030201E.BL</t>
-        </is>
-      </c>
-    </row>
-    <row r="2"/>
+    <row r="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
new pos in DB 29032021
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,7 +424,60 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>D5-PFSC35-38A-190</t>
+          <t>B59840C0120A070</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>B59840C0120A070</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Термистор PTC; 230В; Темп: 0÷60°C; Темп.срабат.предохр: 120°C; 6Ом</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>0.00359</v>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/v7/_cdn_/E5/8A/70/00/0/501854_1.jpg?width=640&amp;height=480&amp;wat=1&amp;wat_url=_tme-wrk_%2Ftme_new.png&amp;wat_scale=100p&amp;ci_sign=94006b95ba11b4f1017f94e5495383dcd6f7f186</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/b59840c0120a070/termistory-ptc/epcos/</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>{'Тип датчика': 'термистор PTC', 'Максимальное напряжение': '230В', 'Рабочая температура': '0...60°C', 'Температура срабатывания предохранителя': '120°C', 'Максимальное сопротивление': '6Ом'}</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/a747cef2cf3909cffc87d9417091b0e6/OC_Leaded_230V_C_B598.pdf</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Переменные резисторы типа терморезисторы (электрическое сопротивление изменяется в зависимости от температуры). Максимальное напряжение 230 В, Рабочая температура 0...60°C, максимальный порог чувствительности при температуре 120°C, Максимальное сопротивление 6 Ом, предназначены для использования в радиоэлектронном оборудовании общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Тип датчика термистор PTC</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>EPCOS</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>B59840C0120A070</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
git add -A! NEW ASSEMBLY
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L5"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,75 +424,248 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>MX25R3235FZBIL0</t>
+          <t>UDA1361TS/N1</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>UDA1361TS/N1</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>АЦП; Каналы: 1; 24бит; 110квыб./с; 2,4÷3,6В; SSOP16</t>
+        </is>
+      </c>
+      <c r="D1" t="n">
+        <v>7.1e-05</v>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/v7/_cdn_/09/DC/00/00/0/52624_1.jpg?width=640&amp;height=480&amp;wat=1&amp;wat_url=_tme-wrk_%2Ftme_new.png&amp;wat_scale=100p&amp;ci_sign=b7f51d47faec248dda86032605af027a8f164846</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/uda1361ts_n1/preobrazovateli-a-d-mikroskhemy/nxp/uda1361ts-n1-112/</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>{'Тип микросхемы': 'АЦП', 'Кол-во каналов': '2', 'Разрешение преобразователя': '24бит', 'Частота обновления': '110квыб./с', 'Корпус': 'SSOP16', 'Монтаж': 'SMD', 'Интерфейс': 'I2S', 'Характеристики интегральных схем': 'stereo', 'Частота': '96кГц', 'Напряжение питания': '2,4...3,6В DC'}</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/caa190e31c8e714c0e9d5eed22619b2e/UDA1361TS-N1-DTE.pdf</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Тип микросхемы АЦП</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>NXP</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>UDA1361TS/N1,112</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CD4011BMT</t>
+          <t>R2K150-AC01-15</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FM4934W</t>
+          <t>BQ27441DRZT-G1A</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BQ27441DRZT-G1A</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Система контроля; контроллер заряда аккумуляторов; SON12</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>0.00017</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/v7/_cdn_/27/67/B0/00/0/751218_1.jpg?width=640&amp;height=480&amp;wat=1&amp;wat_url=_tme-wrk_%2Ftme_new.png&amp;wat_scale=100p&amp;ci_sign=f0ec52a3f4b002933ece394ec659d28b3fdbd260</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/bq27441drzt-g1a/kontrollery-batarei-i-akkumuliat-skhemy/texas-instruments/</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>{'Тип микросхемы': 'система контроля', 'Вид микросхемы': 'контроллер заряда аккумуляторов', 'Корпус': 'SON12', 'Выходное напряжение': '4,2В', 'Интерфейс': 'I2C', 'Рабочая температура': '-40...85°C', 'Монтаж': 'SMD', 'Количество аккумуляторов': '1 x Li-Ion / Li-Po'}</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Интегральные монолитные схемы — регулятор заряда аккумуляторов. Корпус SON12, Выходное напряжение 4,2В, Интерфейс I2C, Рабочая температура -40...85°C, Монтаж на поверхность печатной платы, Количество аккумуляторов 1 x Li-Ion / Li-Po, предназначены для монтажа на печатную плату радиоэлектронного оборудования общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Тип микросхемы система контроля</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>TEXAS INSTRUMENTS</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>BQ27441DRZT-G1A</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>ES1G</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>ES1G-13-F</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Диод: импульсный; SMD; 400В; 1А; 25нс; Упаковка: бобина,лента; SMA</t>
-        </is>
-      </c>
-      <c r="D4" t="n">
-        <v>0.0001</v>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>//www.tme.eu/ru/details/es1g-13-f/universalnye-diody-smd/diodes-incorporated/</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>{'Тип диода': 'импульсный', 'Монтаж': 'SMD', 'Обратное напряжение макс.': '400В', 'Прямой ток': '1А', 'Время готовности': '25нс', 'Конструкция диода': 'одиночный диод', 'Характеристики полупроводниковых элементов': 'супер-быстрое переключение', 'Емкость': '20пФ', 'Вид упаковки': 'лента', 'Корпус': 'SMA', 'Падение напряжения макс.': '1,25В', 'Импульсный ток': '30А'}</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Диоды полупроводниковые, импульсные. Обратное напряжение до 400В, падение напряжения до 1,25В, Прямой ток 1А, Импульсный ток 30А, тип корпуса SMA, монтаж на поверхность печатной платы, рабочая температура от -40 до 85°С. Используются для монтажа в радиоэлектронных устройствах общепромышленного применения.</t>
-        </is>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Тип диода импульсный</t>
-        </is>
-      </c>
-      <c r="K4" t="inlineStr">
-        <is>
-          <t>DIODES INCORPORATED</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>ES1G-13-F</t>
+          <t>MAX7317AEE+</t>
         </is>
       </c>
     </row>
-    <row r="5"/>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>IRFR5305PBF</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>IRFR5305PBF</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Транзистор: P-MOSFET; полевой; -55В; -28А; 89Вт; DPAK</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.00032</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/v7/_cdn_/16/7E/00/00/0/59233_1.jpg?width=640&amp;height=480&amp;wat=1&amp;wat_url=_tme-wrk_%2Ftme_new.png&amp;wat_scale=100p&amp;ci_sign=85a92da44426a86680dc5a939d6fe19e96293048</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/irfr5305pbf/tranzistory-s-kanalom-p-smd/infineon-irf/</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>{'Тип транзистора': 'P-MOSFET', 'Технология': 'HEXFET®', 'Полярность': 'полевой', 'Напряжение сток-исток': '-55В', 'Ток стока': '-28А', 'Рассеиваемая мощность': '89Вт', 'Корпус': 'DPAK', 'Напряжение затвор-исток': '±20В', 'Сопротивление в открытом состоянии': '65мОм', 'Монтаж': 'SMD', 'Заряд затвора': '42нC', 'Вид канала': 'обогащенный'}</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/c3ef49bf7438fe933f8717d1acbf6b87/irfr5305.pdf</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Кремниевые МОП-транзисторы с P-канальной структурой. Тип транзистора P-MOSFET, Технология HEXFET, Полярность полевой, Напряжение сток-исток -55В, Ток стока -28А, Рассеиваемая мощность 89Вт, Корпус DPAK, Напряжение затвор-исток +\- 20В, Сопротивление в открытом состоянии 65мОм, Монтаж на поверхность печатной платы, Заряд затвора 42нC, рабочие температуры от -40 до 85°С, предназначены для использования в радиоэлектронном оборудовании промышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>Тип транзистора P-MOSFET</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Infineon (IRF)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>IRFR5305PBF</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>0456020.ER</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>0456020.ER</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Предохранитель: плавкая вставка; быстродействующий; 20А; 125ВAC</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://ce8dc832c.cloudimg.io/v7/_cdn_/0D/DD/00/00/0/56784_1.jpg?width=640&amp;height=480&amp;wat=1&amp;wat_url=_tme-wrk_%2Ftme_new.png&amp;wat_scale=100p&amp;ci_sign=5eda84b4c4f9995ae1e3ee2216ad2332ca0cafc7</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>//www.tme.eu/ru/details/0456020.er/predokhraniteli-smd-ostalnye/littelfuse/</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>{'Тип предохранителя': 'плавкая вставка', 'Характеристика предохранителя': 'быстрый', 'Ток отключения': '100А', 'Номинальный ток': '20А', 'Номинальное напряжение': '125В AC', 'Монтаж': 'SMD', 'Вид предохранителя': 'керамический', 'Размер предохранителя': '10,1x3,12x3,12мм', 'Характеристика отключения': '2I&lt;sub&gt;n&lt;/sub&gt;: макс 60с', 'Материал контакта': 'латунь', 'Покрытие контакта': 'посеребренные'}</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>https://www.tme.eu/Document/a32a0db7e672d04a049bb50c11ca8186/0456020.ER.pdf</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Предохранители плавкие. Характеристика предохранителя быстрый, Номинальный ток 20А, Номинальное напряжение 125В переменного тока, Монтаж на поверхность печатной платы, Вид предохранителя керамический, Размер предохранителя 10,1x3,12x3,12мм, Материал контакта латунь. Предназначены для использования в радиоэлектронном оборудовании общепромышленного назначения.</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>Тип предохранителя плавкая вставка</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>LITTELFUSE</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>0456020.ER</t>
+        </is>
+      </c>
+    </row>
+    <row r="7"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
06082021 new in DB
</commit_message>
<xml_diff>
--- a/productdata.xlsx
+++ b/productdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,55 +424,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>FIX-MWS-19</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>FIX-MWS-19</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>Держатель с защелкой; полиамид; Внутр.шир: 9мм; натуральный</t>
-        </is>
-      </c>
-      <c r="D1" t="n">
-        <v>0.0002</v>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>https://ce8dc832c.cloudimg.io/v7/_cdn_/58/62/80/00/0/534149_1.jpg?width=640&amp;height=480&amp;wat=1&amp;wat_url=_tme-wrk_%2Ftme_new.png&amp;wat_scale=100p&amp;ci_sign=b8fcde05fe971794863430c91173e54beded4013</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>//www.tme.eu/ru/details/fix-mws-19/derzhateli-skoby-dlia-kabelei/fix-fasten/</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>{'Тип кабельных аксессуаров': 'держатель с защелкой', 'Материал корпуса': 'полиамид', 'Внутренняя ширина': '9мм', 'Цвет': 'натуральный', 'Класс горючести': 'UL94V-2', 'Размер монтажного отверстия': 'Ø3,5мм', 'Толщина панели': '0,8...1,2мм', 'Применение кабельных аксессуаров': 'для крепления проводов'}</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>https://www.tme.eu/Document/59903bd0a113e957755812e6a3096c56/FIX-MWS.pdf</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Изделия изготовленные из пластмассы — клипсы для крепления кабельной стяжки. Защелкивающегося типа, Материал полиамид, Внутренняя ширина 9мм, Цвет светло-серый, Размер монтажного отверстия диам. 3,5мм, Толщина панели 0,8...1,2мм. Предназначены для совместного использования с кабельными хомутами, для монтажа проводников.</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Тип кабельных аксессуаров держатель с защелкой</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
-        <is>
-          <t>FIX&amp;FASTEN</t>
+          <t>K9F1G08U0B-PIB0</t>
         </is>
       </c>
     </row>

</xml_diff>